<commit_message>
Letra J: agrega letra-español-gnabere-oracion
</commit_message>
<xml_diff>
--- a/src/data/plantillaTerminos.xlsx
+++ b/src/data/plantillaTerminos.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\traducto-ngabere\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7935" windowHeight="4575" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7935" windowHeight="4575" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="letraA" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="letraCH" sheetId="3" r:id="rId3"/>
     <sheet name="letraD4" sheetId="4" r:id="rId4"/>
     <sheet name="letraGW" sheetId="5" r:id="rId5"/>
+    <sheet name="letraJ" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="1184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1610" uniqueCount="1248">
   <si>
     <t>id</t>
   </si>
@@ -3539,59 +3540,336 @@
     <t xml:space="preserve">Rana </t>
   </si>
   <si>
-    <t xml:space="preserve">Gwa ye mrende </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ani gwä sribire </t>
-  </si>
-  <si>
-    <t>Jagwe gwä ngwäne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blite gwaire ngäbere </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Juben gwairebe dötrö </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gwara  möin deme </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jagwe gwi nete </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gwreta ye turi mägwe  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ese pescado es del mar </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vamos ya a trabajar </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Venga de inmediato </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hablen juntos en ngäbere </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bañasen rápidos todos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Escarbe despacio la lombriz </t>
-  </si>
-  <si>
     <t xml:space="preserve">Venga aquí adentro de la casa. </t>
   </si>
   <si>
     <t xml:space="preserve">Usted vio a una rana.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ese pescado es del mar. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vamos ya a trabajar. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venga de inmediato. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hablen juntos en ngäbere. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bañasen rápidos todos. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Escarbe despacio la lombriz. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gwreta ye turi mägwe.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jagwe gwi nete. </t>
+  </si>
+  <si>
+    <t>Gwara  möin deme.</t>
+  </si>
+  <si>
+    <t>texto_gnabere.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gwa ye mrende. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ani gwä sribire. </t>
+  </si>
+  <si>
+    <t>Jagwe gwä ngwäne.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blite gwaire ngäbere. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juben gwairebe dötrö. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ja </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>jä</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Jadengä </t>
+  </si>
+  <si>
+    <t xml:space="preserve">jadabare </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">jagani </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">jadagai </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jadugue </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>jadugabare</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">jadugai </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">jadugani </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jagain </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jamete </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jametai </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">jametabare </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Jägue </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jagwe </t>
+  </si>
+  <si>
+    <t>Jagwre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verbo reflexivo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piedra </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jugar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jugaron </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jugó </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jugará </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dormir </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Durmieron </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dormirán </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dormido </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Competir </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pelear </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pelearan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pelearon </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jalar </t>
+  </si>
+  <si>
+    <t>Venga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ani jagain gwa kite. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vamos en la tarde a jugar. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ellos jugaron conmigo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">El jugara con nosotros. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ellos durmieron cerca de él. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vieron a Nei dormido.  </t>
+  </si>
+  <si>
+    <t>Hagamos competencia para pescar.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voy a ir a jalar leña. </t>
+  </si>
+  <si>
+    <t>Él ya se fue a dormir.</t>
+  </si>
+  <si>
+    <t>Yo me voy a dormir temprano.</t>
+  </si>
+  <si>
+    <t>Él estaba ayer peleando.</t>
+  </si>
+  <si>
+    <t>Él va a Pelearan conmigo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esos dos caballos pelearon. </t>
+  </si>
+  <si>
+    <t>Venga siéntese aquí.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jä ye bä ngwen. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ani Jadengä dere. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kwetre jadagabare tibe. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ni se jadagani kuin. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ni se jadagai nibe. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kugwe niguira jadugue. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kwetre jadugabare ken. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tigwe jadugai derebe. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nei tuani jadugani. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kwe nämä jamete jädrin. </t>
+  </si>
+  <si>
+    <t>Ni segwe jametai tibe.</t>
+  </si>
+  <si>
+    <t>Mädä krobu ye jametabare.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ti näin ngi jägue. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jagwe tägue nete. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esa piedra es de color blanco. </t>
+  </si>
+  <si>
+    <t>El jugo bien.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3725,6 +4003,26 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -4068,9 +4366,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -14485,19 +14787,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
@@ -14519,7 +14821,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>1179</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -14551,7 +14853,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>153</v>
+        <v>282</v>
       </c>
       <c r="B2" t="s">
         <v>1153</v>
@@ -14560,10 +14862,10 @@
         <v>1161</v>
       </c>
       <c r="D2" t="s">
-        <v>1168</v>
+        <v>1180</v>
       </c>
       <c r="E2" t="s">
-        <v>1176</v>
+        <v>1170</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
@@ -14591,6 +14893,9 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>283</v>
+      </c>
       <c r="B3" t="s">
         <v>1154</v>
       </c>
@@ -14598,13 +14903,16 @@
         <v>502</v>
       </c>
       <c r="D3" t="s">
-        <v>1169</v>
+        <v>1181</v>
       </c>
       <c r="E3" t="s">
-        <v>1177</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>284</v>
+      </c>
       <c r="B4" t="s">
         <v>1155</v>
       </c>
@@ -14612,13 +14920,16 @@
         <v>1162</v>
       </c>
       <c r="D4" t="s">
-        <v>1170</v>
+        <v>1182</v>
       </c>
       <c r="E4" t="s">
-        <v>1178</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>285</v>
+      </c>
       <c r="B5" t="s">
         <v>1156</v>
       </c>
@@ -14626,13 +14937,16 @@
         <v>1163</v>
       </c>
       <c r="D5" t="s">
-        <v>1171</v>
+        <v>1183</v>
       </c>
       <c r="E5" t="s">
-        <v>1179</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>286</v>
+      </c>
       <c r="B6" t="s">
         <v>1157</v>
       </c>
@@ -14640,13 +14954,16 @@
         <v>1164</v>
       </c>
       <c r="D6" t="s">
-        <v>1172</v>
+        <v>1184</v>
       </c>
       <c r="E6" t="s">
-        <v>1180</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>287</v>
+      </c>
       <c r="B7" t="s">
         <v>1158</v>
       </c>
@@ -14654,13 +14971,16 @@
         <v>1165</v>
       </c>
       <c r="D7" t="s">
-        <v>1173</v>
+        <v>1178</v>
       </c>
       <c r="E7" t="s">
-        <v>1181</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>288</v>
+      </c>
       <c r="B8" t="s">
         <v>1159</v>
       </c>
@@ -14668,13 +14988,16 @@
         <v>1166</v>
       </c>
       <c r="D8" t="s">
-        <v>1174</v>
+        <v>1177</v>
       </c>
       <c r="E8" t="s">
-        <v>1182</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>289</v>
+      </c>
       <c r="B9" t="s">
         <v>1160</v>
       </c>
@@ -14682,10 +15005,396 @@
         <v>1167</v>
       </c>
       <c r="D9" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="E9" t="s">
-        <v>1183</v>
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E10" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>290</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1202</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1246</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" t="s">
+        <v>735</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>43867.470242997682</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>291</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1203</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1232</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1219</v>
+      </c>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>292</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1204</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1220</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>293</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1205</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1234</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1247</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>294</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1206</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1235</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1221</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>295</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1207</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1236</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1226</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>296</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1208</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1237</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1222</v>
+      </c>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>297</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1209</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1227</v>
+      </c>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>298</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1210</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1239</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1223</v>
+      </c>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>299</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1240</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1224</v>
+      </c>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>300</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1212</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1218</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1228</v>
+      </c>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>301</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1241</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1229</v>
+      </c>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>302</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1214</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1242</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1230</v>
+      </c>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>303</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1198</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1243</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1225</v>
+      </c>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>304</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1216</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1244</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1231</v>
+      </c>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>305</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1217</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1245</v>
+      </c>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>306</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Plantilla términos actualizada y variable que captura dispositivo usado
</commit_message>
<xml_diff>
--- a/src/data/plantillaTerminos.xlsx
+++ b/src/data/plantillaTerminos.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\traducto-ngabere\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prueba\www\traducto-ngabere\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7935" windowHeight="4575" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7935" windowHeight="4575" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="letraA" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2317" uniqueCount="1763">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2320" uniqueCount="1763">
   <si>
     <t>id</t>
   </si>
@@ -12737,7 +12737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -13145,8 +13145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M77"/>
   <sheetViews>
-    <sheetView topLeftCell="E57" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13217,15 +13217,12 @@
       <c r="C2" t="s">
         <v>780</v>
       </c>
-      <c r="E2" t="s">
-        <v>824</v>
-      </c>
       <c r="F2" t="s">
         <v>17</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G33" si="0">CONCATENATE("subidos/imagenes/",A2,"_letra_gw.png")</f>
-        <v>subidos/imagenes/290_letra_gw.png</v>
+        <f>CONCATENATE("subidos/imagenes/",A2,"_letra_j.png")</f>
+        <v>subidos/imagenes/290_letra_j.png</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -13260,14 +13257,14 @@
         <v>810</v>
       </c>
       <c r="E3" t="s">
-        <v>797</v>
+        <v>824</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" si="0"/>
-        <v>subidos/imagenes/291_letra_gw.png</v>
+        <f t="shared" ref="G3:G66" si="0">CONCATENATE("subidos/imagenes/",A3,"_letra_j.png")</f>
+        <v>subidos/imagenes/291_letra_j.png</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -13302,14 +13299,14 @@
         <v>811</v>
       </c>
       <c r="E4" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/292_letra_gw.png</v>
+        <v>subidos/imagenes/292_letra_j.png</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -13344,14 +13341,14 @@
         <v>812</v>
       </c>
       <c r="E5" t="s">
-        <v>825</v>
+        <v>798</v>
       </c>
       <c r="F5" t="s">
         <v>17</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/293_letra_gw.png</v>
+        <v>subidos/imagenes/293_letra_j.png</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -13386,14 +13383,14 @@
         <v>813</v>
       </c>
       <c r="E6" t="s">
-        <v>799</v>
+        <v>825</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/294_letra_gw.png</v>
+        <v>subidos/imagenes/294_letra_j.png</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -13428,14 +13425,14 @@
         <v>814</v>
       </c>
       <c r="E7" t="s">
-        <v>804</v>
+        <v>799</v>
       </c>
       <c r="F7" t="s">
         <v>17</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/295_letra_gw.png</v>
+        <v>subidos/imagenes/295_letra_j.png</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -13470,14 +13467,14 @@
         <v>815</v>
       </c>
       <c r="E8" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
       <c r="F8" t="s">
         <v>17</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/296_letra_gw.png</v>
+        <v>subidos/imagenes/296_letra_j.png</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -13512,14 +13509,14 @@
         <v>816</v>
       </c>
       <c r="E9" t="s">
-        <v>805</v>
+        <v>800</v>
       </c>
       <c r="F9" t="s">
         <v>17</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/297_letra_gw.png</v>
+        <v>subidos/imagenes/297_letra_j.png</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -13554,14 +13551,14 @@
         <v>817</v>
       </c>
       <c r="E10" t="s">
-        <v>801</v>
+        <v>805</v>
       </c>
       <c r="F10" t="s">
         <v>17</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/298_letra_gw.png</v>
+        <v>subidos/imagenes/298_letra_j.png</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -13596,14 +13593,14 @@
         <v>818</v>
       </c>
       <c r="E11" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="F11" t="s">
         <v>17</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/299_letra_gw.png</v>
+        <v>subidos/imagenes/299_letra_j.png</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -13638,14 +13635,14 @@
         <v>796</v>
       </c>
       <c r="E12" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="F12" t="s">
         <v>17</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/300_letra_gw.png</v>
+        <v>subidos/imagenes/300_letra_j.png</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -13680,14 +13677,14 @@
         <v>819</v>
       </c>
       <c r="E13" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/301_letra_gw.png</v>
+        <v>subidos/imagenes/301_letra_j.png</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -13722,14 +13719,14 @@
         <v>820</v>
       </c>
       <c r="E14" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="F14" t="s">
         <v>17</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/302_letra_gw.png</v>
+        <v>subidos/imagenes/302_letra_j.png</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -13764,14 +13761,14 @@
         <v>821</v>
       </c>
       <c r="E15" t="s">
-        <v>803</v>
+        <v>808</v>
       </c>
       <c r="F15" t="s">
         <v>17</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/303_letra_gw.png</v>
+        <v>subidos/imagenes/303_letra_j.png</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -13806,14 +13803,14 @@
         <v>822</v>
       </c>
       <c r="E16" t="s">
-        <v>809</v>
+        <v>803</v>
       </c>
       <c r="F16" t="s">
         <v>17</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/304_letra_gw.png</v>
+        <v>subidos/imagenes/304_letra_j.png</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -13847,12 +13844,15 @@
       <c r="D17" t="s">
         <v>823</v>
       </c>
+      <c r="E17" t="s">
+        <v>809</v>
+      </c>
       <c r="F17" t="s">
         <v>17</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/305_letra_gw.png</v>
+        <v>subidos/imagenes/305_letra_j.png</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -13880,12 +13880,21 @@
       <c r="B18" t="s">
         <v>779</v>
       </c>
+      <c r="C18" t="s">
+        <v>795</v>
+      </c>
+      <c r="D18" t="s">
+        <v>823</v>
+      </c>
+      <c r="E18" t="s">
+        <v>809</v>
+      </c>
       <c r="F18" t="s">
         <v>17</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/306_letra_gw.png</v>
+        <v>subidos/imagenes/306_letra_j.png</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -13927,7 +13936,7 @@
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/307_letra_gw.png</v>
+        <v>subidos/imagenes/307_letra_j.png</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -13969,7 +13978,7 @@
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/308_letra_gw.png</v>
+        <v>subidos/imagenes/308_letra_j.png</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -14011,7 +14020,7 @@
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/309_letra_gw.png</v>
+        <v>subidos/imagenes/309_letra_j.png</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -14053,7 +14062,7 @@
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/310_letra_gw.png</v>
+        <v>subidos/imagenes/310_letra_j.png</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -14095,7 +14104,7 @@
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/311_letra_gw.png</v>
+        <v>subidos/imagenes/311_letra_j.png</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -14137,7 +14146,7 @@
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/312_letra_gw.png</v>
+        <v>subidos/imagenes/312_letra_j.png</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -14179,7 +14188,7 @@
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/313_letra_gw.png</v>
+        <v>subidos/imagenes/313_letra_j.png</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -14221,7 +14230,7 @@
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/314_letra_gw.png</v>
+        <v>subidos/imagenes/314_letra_j.png</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -14263,7 +14272,7 @@
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/315_letra_gw.png</v>
+        <v>subidos/imagenes/315_letra_j.png</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -14305,7 +14314,7 @@
       </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/316_letra_gw.png</v>
+        <v>subidos/imagenes/316_letra_j.png</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -14347,7 +14356,7 @@
       </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/317_letra_gw.png</v>
+        <v>subidos/imagenes/317_letra_j.png</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -14389,7 +14398,7 @@
       </c>
       <c r="G30" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/318_letra_gw.png</v>
+        <v>subidos/imagenes/318_letra_j.png</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -14431,7 +14440,7 @@
       </c>
       <c r="G31" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/319_letra_gw.png</v>
+        <v>subidos/imagenes/319_letra_j.png</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -14473,7 +14482,7 @@
       </c>
       <c r="G32" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/320_letra_gw.png</v>
+        <v>subidos/imagenes/320_letra_j.png</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -14515,7 +14524,7 @@
       </c>
       <c r="G33" t="str">
         <f t="shared" si="0"/>
-        <v>subidos/imagenes/321_letra_gw.png</v>
+        <v>subidos/imagenes/321_letra_j.png</v>
       </c>
       <c r="H33">
         <v>1</v>
@@ -14556,8 +14565,8 @@
         <v>17</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" ref="G34:G65" si="1">CONCATENATE("subidos/imagenes/",A34,"_letra_gw.png")</f>
-        <v>subidos/imagenes/322_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/322_letra_j.png</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -14598,8 +14607,8 @@
         <v>17</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/323_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/323_letra_j.png</v>
       </c>
       <c r="H35">
         <v>1</v>
@@ -14640,8 +14649,8 @@
         <v>17</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/324_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/324_letra_j.png</v>
       </c>
       <c r="H36">
         <v>1</v>
@@ -14682,8 +14691,8 @@
         <v>17</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/325_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/325_letra_j.png</v>
       </c>
       <c r="H37">
         <v>1</v>
@@ -14724,8 +14733,8 @@
         <v>17</v>
       </c>
       <c r="G38" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/326_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/326_letra_j.png</v>
       </c>
       <c r="H38">
         <v>1</v>
@@ -14766,8 +14775,8 @@
         <v>17</v>
       </c>
       <c r="G39" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/327_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/327_letra_j.png</v>
       </c>
       <c r="H39">
         <v>1</v>
@@ -14808,8 +14817,8 @@
         <v>17</v>
       </c>
       <c r="G40" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/328_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/328_letra_j.png</v>
       </c>
       <c r="H40">
         <v>1</v>
@@ -14850,8 +14859,8 @@
         <v>17</v>
       </c>
       <c r="G41" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/329_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/329_letra_j.png</v>
       </c>
       <c r="H41">
         <v>1</v>
@@ -14892,8 +14901,8 @@
         <v>17</v>
       </c>
       <c r="G42" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/330_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/330_letra_j.png</v>
       </c>
       <c r="H42">
         <v>1</v>
@@ -14934,8 +14943,8 @@
         <v>17</v>
       </c>
       <c r="G43" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/331_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/331_letra_j.png</v>
       </c>
       <c r="H43">
         <v>1</v>
@@ -14976,8 +14985,8 @@
         <v>17</v>
       </c>
       <c r="G44" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/332_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/332_letra_j.png</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -15018,8 +15027,8 @@
         <v>17</v>
       </c>
       <c r="G45" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/333_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/333_letra_j.png</v>
       </c>
       <c r="H45">
         <v>1</v>
@@ -15060,8 +15069,8 @@
         <v>17</v>
       </c>
       <c r="G46" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/334_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/334_letra_j.png</v>
       </c>
       <c r="H46">
         <v>1</v>
@@ -15102,8 +15111,8 @@
         <v>17</v>
       </c>
       <c r="G47" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/335_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/335_letra_j.png</v>
       </c>
       <c r="H47">
         <v>1</v>
@@ -15144,8 +15153,8 @@
         <v>17</v>
       </c>
       <c r="G48" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/336_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/336_letra_j.png</v>
       </c>
       <c r="H48">
         <v>1</v>
@@ -15186,8 +15195,8 @@
         <v>17</v>
       </c>
       <c r="G49" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/337_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/337_letra_j.png</v>
       </c>
       <c r="H49">
         <v>1</v>
@@ -15228,8 +15237,8 @@
         <v>17</v>
       </c>
       <c r="G50" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/338_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/338_letra_j.png</v>
       </c>
       <c r="H50">
         <v>1</v>
@@ -15270,8 +15279,8 @@
         <v>17</v>
       </c>
       <c r="G51" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/339_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/339_letra_j.png</v>
       </c>
       <c r="H51">
         <v>1</v>
@@ -15312,8 +15321,8 @@
         <v>17</v>
       </c>
       <c r="G52" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/340_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/340_letra_j.png</v>
       </c>
       <c r="H52">
         <v>1</v>
@@ -15354,8 +15363,8 @@
         <v>17</v>
       </c>
       <c r="G53" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/341_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/341_letra_j.png</v>
       </c>
       <c r="H53">
         <v>1</v>
@@ -15396,8 +15405,8 @@
         <v>17</v>
       </c>
       <c r="G54" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/342_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/342_letra_j.png</v>
       </c>
       <c r="H54">
         <v>1</v>
@@ -15438,8 +15447,8 @@
         <v>17</v>
       </c>
       <c r="G55" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/343_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/343_letra_j.png</v>
       </c>
       <c r="H55">
         <v>1</v>
@@ -15480,8 +15489,8 @@
         <v>17</v>
       </c>
       <c r="G56" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/344_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/344_letra_j.png</v>
       </c>
       <c r="H56">
         <v>1</v>
@@ -15522,8 +15531,8 @@
         <v>17</v>
       </c>
       <c r="G57" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/345_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/345_letra_j.png</v>
       </c>
       <c r="H57">
         <v>1</v>
@@ -15564,8 +15573,8 @@
         <v>17</v>
       </c>
       <c r="G58" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/346_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/346_letra_j.png</v>
       </c>
       <c r="H58">
         <v>1</v>
@@ -15606,8 +15615,8 @@
         <v>17</v>
       </c>
       <c r="G59" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/347_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/347_letra_j.png</v>
       </c>
       <c r="H59">
         <v>1</v>
@@ -15648,8 +15657,8 @@
         <v>17</v>
       </c>
       <c r="G60" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/348_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/348_letra_j.png</v>
       </c>
       <c r="H60">
         <v>1</v>
@@ -15690,8 +15699,8 @@
         <v>17</v>
       </c>
       <c r="G61" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/349_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/349_letra_j.png</v>
       </c>
       <c r="H61">
         <v>1</v>
@@ -15732,8 +15741,8 @@
         <v>17</v>
       </c>
       <c r="G62" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/350_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/350_letra_j.png</v>
       </c>
       <c r="H62">
         <v>1</v>
@@ -15774,8 +15783,8 @@
         <v>17</v>
       </c>
       <c r="G63" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/351_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/351_letra_j.png</v>
       </c>
       <c r="H63">
         <v>1</v>
@@ -15816,8 +15825,8 @@
         <v>17</v>
       </c>
       <c r="G64" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/352_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/352_letra_j.png</v>
       </c>
       <c r="H64">
         <v>1</v>
@@ -15858,8 +15867,8 @@
         <v>17</v>
       </c>
       <c r="G65" t="str">
-        <f t="shared" si="1"/>
-        <v>subidos/imagenes/353_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/353_letra_j.png</v>
       </c>
       <c r="H65">
         <v>1</v>
@@ -15900,8 +15909,8 @@
         <v>17</v>
       </c>
       <c r="G66" t="str">
-        <f t="shared" ref="G66:G77" si="2">CONCATENATE("subidos/imagenes/",A66,"_letra_gw.png")</f>
-        <v>subidos/imagenes/354_letra_gw.png</v>
+        <f t="shared" si="0"/>
+        <v>subidos/imagenes/354_letra_j.png</v>
       </c>
       <c r="H66">
         <v>1</v>
@@ -15942,8 +15951,8 @@
         <v>17</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" si="2"/>
-        <v>subidos/imagenes/355_letra_gw.png</v>
+        <f t="shared" ref="G67:G77" si="1">CONCATENATE("subidos/imagenes/",A67,"_letra_j.png")</f>
+        <v>subidos/imagenes/355_letra_j.png</v>
       </c>
       <c r="H67">
         <v>1</v>
@@ -15984,8 +15993,8 @@
         <v>17</v>
       </c>
       <c r="G68" t="str">
-        <f t="shared" si="2"/>
-        <v>subidos/imagenes/356_letra_gw.png</v>
+        <f t="shared" si="1"/>
+        <v>subidos/imagenes/356_letra_j.png</v>
       </c>
       <c r="H68">
         <v>1</v>
@@ -16026,8 +16035,8 @@
         <v>17</v>
       </c>
       <c r="G69" t="str">
-        <f t="shared" si="2"/>
-        <v>subidos/imagenes/357_letra_gw.png</v>
+        <f t="shared" si="1"/>
+        <v>subidos/imagenes/357_letra_j.png</v>
       </c>
       <c r="H69">
         <v>1</v>
@@ -16068,8 +16077,8 @@
         <v>17</v>
       </c>
       <c r="G70" t="str">
-        <f t="shared" si="2"/>
-        <v>subidos/imagenes/358_letra_gw.png</v>
+        <f t="shared" si="1"/>
+        <v>subidos/imagenes/358_letra_j.png</v>
       </c>
       <c r="H70">
         <v>1</v>
@@ -16110,8 +16119,8 @@
         <v>17</v>
       </c>
       <c r="G71" t="str">
-        <f t="shared" si="2"/>
-        <v>subidos/imagenes/359_letra_gw.png</v>
+        <f t="shared" si="1"/>
+        <v>subidos/imagenes/359_letra_j.png</v>
       </c>
       <c r="H71">
         <v>1</v>
@@ -16152,8 +16161,8 @@
         <v>17</v>
       </c>
       <c r="G72" t="str">
-        <f t="shared" si="2"/>
-        <v>subidos/imagenes/360_letra_gw.png</v>
+        <f t="shared" si="1"/>
+        <v>subidos/imagenes/360_letra_j.png</v>
       </c>
       <c r="H72">
         <v>1</v>
@@ -16194,8 +16203,8 @@
         <v>17</v>
       </c>
       <c r="G73" t="str">
-        <f t="shared" si="2"/>
-        <v>subidos/imagenes/361_letra_gw.png</v>
+        <f t="shared" si="1"/>
+        <v>subidos/imagenes/361_letra_j.png</v>
       </c>
       <c r="H73">
         <v>1</v>
@@ -16236,8 +16245,8 @@
         <v>17</v>
       </c>
       <c r="G74" t="str">
-        <f t="shared" si="2"/>
-        <v>subidos/imagenes/362_letra_gw.png</v>
+        <f t="shared" si="1"/>
+        <v>subidos/imagenes/362_letra_j.png</v>
       </c>
       <c r="H74">
         <v>1</v>
@@ -16278,8 +16287,8 @@
         <v>17</v>
       </c>
       <c r="G75" t="str">
-        <f t="shared" si="2"/>
-        <v>subidos/imagenes/363_letra_gw.png</v>
+        <f t="shared" si="1"/>
+        <v>subidos/imagenes/363_letra_j.png</v>
       </c>
       <c r="H75">
         <v>1</v>
@@ -16320,8 +16329,8 @@
         <v>17</v>
       </c>
       <c r="G76" t="str">
-        <f t="shared" si="2"/>
-        <v>subidos/imagenes/364_letra_gw.png</v>
+        <f t="shared" si="1"/>
+        <v>subidos/imagenes/364_letra_j.png</v>
       </c>
       <c r="H76">
         <v>1</v>
@@ -16362,8 +16371,8 @@
         <v>17</v>
       </c>
       <c r="G77" t="str">
-        <f t="shared" si="2"/>
-        <v>subidos/imagenes/365_letra_gw.png</v>
+        <f t="shared" si="1"/>
+        <v>subidos/imagenes/365_letra_j.png</v>
       </c>
       <c r="H77">
         <v>1</v>
@@ -16394,7 +16403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M185"/>
   <sheetViews>
-    <sheetView topLeftCell="E178" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E178" workbookViewId="0">
       <selection activeCell="J191" sqref="J191"/>
     </sheetView>
   </sheetViews>

</xml_diff>